<commit_message>
test: Update tests after fixing TMFA
</commit_message>
<xml_diff>
--- a/matlab_code/tests/ensembleFxns/testFiles/toy_model1_random2_linprog.xlsx
+++ b/matlab_code/tests/ensembleFxns/testFiles/toy_model1_random2_linprog.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">Model name</t>
   </si>
   <si>
-    <t xml:space="preserve">toy_model1_random2</t>
+    <t xml:space="preserve">toy_model1_random2_linprog</t>
   </si>
   <si>
     <t xml:space="preserve">Sampling mode (GRASP or rejection)</t>
@@ -609,7 +609,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="B3 A8"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -634,7 +634,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>45</v>
       </c>
@@ -642,16 +642,18 @@
         <v>-22.0149320730417</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>1.10350536706976</v>
+        <f aca="false">ABS(0.15*B2)</f>
+        <v>3.30223981095625</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>-22.0149320730417</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>1.10350536706976</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">ABS(0.15*D2)</f>
+        <v>3.30223981095625</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>46</v>
       </c>
@@ -659,16 +661,18 @@
         <v>0.285369137837419</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>2.12397436954052E-007</v>
+        <f aca="false">ABS(0.15*B3)</f>
+        <v>0.0428053706756129</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0.285369137837419</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>2.12397436954052E-007</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">ABS(0.15*D3)</f>
+        <v>0.0428053706756129</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>47</v>
       </c>
@@ -676,16 +680,18 @@
         <v>0.0578197638950879</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>3.18755368558865E-009</v>
+        <f aca="false">ABS(0.15*B4)</f>
+        <v>0.00867296458426318</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0.0578197638950879</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>3.18755368558865E-009</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">ABS(0.15*D4)</f>
+        <v>0.00867296458426318</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>48</v>
       </c>
@@ -693,16 +699,18 @@
         <v>-0.00439408376660814</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>3.33787220043099E-011</v>
+        <f aca="false">ABS(0.15*B5)</f>
+        <v>0.000659112564991221</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>-0.00439408376660814</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>3.33787220043099E-011</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">ABS(0.15*D5)</f>
+        <v>0.000659112564991221</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>49</v>
       </c>
@@ -710,16 +718,18 @@
         <v>6.84865633256387</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>2.00430304742416E-005</v>
+        <f aca="false">ABS(0.15*B6)</f>
+        <v>1.02729844988458</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>6.84865633256387</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>2.00430304742416E-005</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">ABS(0.15*D6)</f>
+        <v>1.02729844988458</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>50</v>
       </c>
@@ -727,13 +737,15 @@
         <v>-0.00242684925806694</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>6.60284204552005E-011</v>
+        <f aca="false">ABS(0.15*B7)</f>
+        <v>0.000364027388710041</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>-0.00242684925806694</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>6.60284204552005E-011</v>
+        <f aca="false">ABS(0.15*D7)</f>
+        <v>0.000364027388710041</v>
       </c>
     </row>
   </sheetData>
@@ -755,7 +767,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B3 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -978,7 +990,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B3 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1299,7 +1311,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="1" sqref="B3 L2"/>
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1612,7 +1624,7 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B3 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2549,7 +2561,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="B3 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2871,7 +2883,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H23" activeCellId="1" sqref="B3 H23"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3056,7 +3068,7 @@
   <dimension ref="A2:A15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="B3 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3153,7 +3165,7 @@
   <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="B3 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3285,7 +3297,7 @@
   <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="B3 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3417,7 +3429,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B3 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3598,7 +3610,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="1" sqref="B3 H13"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>